<commit_message>
Changes to LCOE and additional scenarios
CODE:
- Some variables were overwritten by exogenous ones (obtained from E3ME); these are now calculated endogenous
- The LCOE for decision making (METC) did not use the load factor of the marginal unit (MCFC); it does now (only applies to VRE due to the CSC routine)
- Added an LCOE variable that excludes storage costs (MWCB) to isolate the learning-by-doing effect

INPUTS:
- Added scenarios S0/1/2_low_sub_freq. These contain altered substitution frequencies (MEWA) for the onshore/offshore/solar  PV pairs to reduce direct competition effect.
</commit_message>
<xml_diff>
--- a/Utilities/titles/VariableListing.xlsx
+++ b/Utilities/titles/VariableListing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ximin\Documents\GitHub\FTT_StandAlone_v0.8\Utilities\titles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cambridgeeconometrics-my.sharepoint.com/personal/pv_camecon_com/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191AE843-71E2-4AD2-972B-67BDE868AD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{191AE843-71E2-4AD2-972B-67BDE868AD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B389DA8-A540-4B62-A504-3F32AB0B4FA1}"/>
   <bookViews>
-    <workbookView xWindow="-130" yWindow="10690" windowWidth="19420" windowHeight="10300" xr2:uid="{3966A5EA-18B5-40FC-82B6-8DC341B5B05B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3966A5EA-18B5-40FC-82B6-8DC341B5B05B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3316" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="719">
   <si>
     <t>Variable name</t>
   </si>
@@ -2188,6 +2188,12 @@
   </si>
   <si>
     <t>FTT-Transport Hydrogen blending mandate</t>
+  </si>
+  <si>
+    <t>MWCB</t>
+  </si>
+  <si>
+    <t>Bare LCOE w/o storage cost component</t>
   </si>
 </sst>
 </file>
@@ -2556,13 +2562,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5694E675-77F6-4F54-A793-A54451BF0049}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:N327"/>
+  <dimension ref="A1:N328"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14330,6 +14336,50 @@
         <v>36</v>
       </c>
     </row>
+    <row r="328" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>717</v>
+      </c>
+      <c r="B328" t="s">
+        <v>718</v>
+      </c>
+      <c r="C328" t="s">
+        <v>190</v>
+      </c>
+      <c r="D328" t="s">
+        <v>29</v>
+      </c>
+      <c r="E328" t="s">
+        <v>11</v>
+      </c>
+      <c r="F328" t="s">
+        <v>17</v>
+      </c>
+      <c r="G328" t="s">
+        <v>8</v>
+      </c>
+      <c r="H328" t="s">
+        <v>31</v>
+      </c>
+      <c r="I328" t="s">
+        <v>9</v>
+      </c>
+      <c r="J328" t="s">
+        <v>9</v>
+      </c>
+      <c r="K328">
+        <v>2001</v>
+      </c>
+      <c r="L328" t="s">
+        <v>9</v>
+      </c>
+      <c r="M328" t="s">
+        <v>233</v>
+      </c>
+      <c r="N328" t="s">
+        <v>233</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L327" xr:uid="{5694E675-77F6-4F54-A793-A54451BF0049}">
     <filterColumn colId="7">

</xml_diff>

<commit_message>
Computing HJEF, halfway done
Start computing HJEF. Have made sure the FU14A/FU14B are correct, but still need to work on the non-heat aspect. Will likely only do it for electricity.
</commit_message>
<xml_diff>
--- a/Utilities/titles/VariableListing.xlsx
+++ b/Utilities/titles/VariableListing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work profile\Documents\GitHub\FTT_StandAlone\Utilities\titles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64002A6-087A-4710-A4E2-8DCABD50D6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F1A958-DA3F-4CC1-802C-B0D80A15EF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{3966A5EA-18B5-40FC-82B6-8DC341B5B05B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3380" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3381" uniqueCount="740">
   <si>
     <t>Variable name</t>
   </si>
@@ -1524,9 +1524,6 @@
     <t>ZEWE</t>
   </si>
   <si>
-    <t>FTT-Fr emissions</t>
-  </si>
-  <si>
     <t>IUD1</t>
   </si>
   <si>
@@ -2257,6 +2254,9 @@
   </si>
   <si>
     <t>FTT-Transport levelised costs with taxes</t>
+  </si>
+  <si>
+    <t>FTT-Fr Emissions</t>
   </si>
 </sst>
 </file>
@@ -2628,10 +2628,10 @@
   <dimension ref="A1:N332"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H303" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H107" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A329" sqref="A329:XFD329"/>
+      <selection pane="bottomRight" activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6270,10 +6270,10 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>715</v>
+      </c>
+      <c r="B89" t="s">
         <v>716</v>
-      </c>
-      <c r="B89" t="s">
-        <v>717</v>
       </c>
       <c r="C89" t="s">
         <v>6</v>
@@ -6311,7 +6311,7 @@
         <v>62</v>
       </c>
       <c r="B90" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C90" t="s">
         <v>193</v>
@@ -7961,6 +7961,9 @@
       <c r="B137" t="s">
         <v>368</v>
       </c>
+      <c r="C137" t="s">
+        <v>35</v>
+      </c>
       <c r="D137" t="s">
         <v>29</v>
       </c>
@@ -8320,13 +8323,13 @@
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
+        <v>717</v>
+      </c>
+      <c r="B151" t="s">
         <v>718</v>
       </c>
-      <c r="B151" t="s">
+      <c r="C151" t="s">
         <v>719</v>
-      </c>
-      <c r="C151" t="s">
-        <v>720</v>
       </c>
       <c r="D151" t="s">
         <v>29</v>
@@ -8349,10 +8352,10 @@
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
+        <v>720</v>
+      </c>
+      <c r="B152" t="s">
         <v>721</v>
-      </c>
-      <c r="B152" t="s">
-        <v>722</v>
       </c>
       <c r="C152" t="s">
         <v>264</v>
@@ -8390,10 +8393,10 @@
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B153" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C153" t="s">
         <v>35</v>
@@ -8408,7 +8411,7 @@
         <v>17</v>
       </c>
       <c r="G153" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="H153" t="s">
         <v>317</v>
@@ -8428,13 +8431,13 @@
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>723</v>
+      </c>
+      <c r="B154" t="s">
         <v>724</v>
       </c>
-      <c r="B154" t="s">
+      <c r="C154" t="s">
         <v>725</v>
-      </c>
-      <c r="C154" t="s">
-        <v>726</v>
       </c>
       <c r="D154" t="s">
         <v>29</v>
@@ -8446,7 +8449,7 @@
         <v>17</v>
       </c>
       <c r="G154" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="H154" t="s">
         <v>317</v>
@@ -8651,7 +8654,7 @@
         <v>396</v>
       </c>
       <c r="B162" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D162" t="s">
         <v>29</v>
@@ -8700,10 +8703,10 @@
         <v>400</v>
       </c>
       <c r="B164" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C164" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D164" t="s">
         <v>29</v>
@@ -8755,10 +8758,10 @@
         <v>403</v>
       </c>
       <c r="B166" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C166" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D166" t="s">
         <v>17</v>
@@ -8813,10 +8816,10 @@
         <v>387</v>
       </c>
       <c r="B168" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C168" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D168" t="s">
         <v>29</v>
@@ -8842,10 +8845,10 @@
         <v>398</v>
       </c>
       <c r="B169" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C169" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D169" t="s">
         <v>29</v>
@@ -8871,10 +8874,10 @@
         <v>389</v>
       </c>
       <c r="B170" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C170" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D170" t="s">
         <v>29</v>
@@ -8900,10 +8903,10 @@
         <v>402</v>
       </c>
       <c r="B171" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C171" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D171" t="s">
         <v>29</v>
@@ -8929,10 +8932,10 @@
         <v>391</v>
       </c>
       <c r="B172" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C172" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D172" t="s">
         <v>29</v>
@@ -8978,10 +8981,10 @@
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>708</v>
+      </c>
+      <c r="B174" t="s">
         <v>709</v>
-      </c>
-      <c r="B174" t="s">
-        <v>710</v>
       </c>
       <c r="D174" t="s">
         <v>17</v>
@@ -9065,10 +9068,10 @@
         <v>392</v>
       </c>
       <c r="B177" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C177" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D177" t="s">
         <v>29</v>
@@ -9091,10 +9094,10 @@
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B178" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D178" t="s">
         <v>29</v>
@@ -9377,10 +9380,10 @@
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
+        <v>712</v>
+      </c>
+      <c r="B189" t="s">
         <v>713</v>
-      </c>
-      <c r="B189" t="s">
-        <v>714</v>
       </c>
       <c r="D189" t="s">
         <v>29</v>
@@ -9507,10 +9510,10 @@
     </row>
     <row r="194" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B194" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C194" t="s">
         <v>35</v>
@@ -9548,10 +9551,10 @@
     </row>
     <row r="195" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B195" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C195" t="s">
         <v>161</v>
@@ -9592,10 +9595,10 @@
     </row>
     <row r="196" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B196" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C196" t="s">
         <v>16</v>
@@ -9633,10 +9636,10 @@
     </row>
     <row r="197" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B197" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C197" t="s">
         <v>16</v>
@@ -9674,10 +9677,10 @@
     </row>
     <row r="198" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B198" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C198" t="s">
         <v>16</v>
@@ -9715,10 +9718,10 @@
     </row>
     <row r="199" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B199" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C199" t="s">
         <v>188</v>
@@ -9753,10 +9756,10 @@
     </row>
     <row r="200" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B200" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C200" t="s">
         <v>263</v>
@@ -9791,10 +9794,10 @@
     </row>
     <row r="201" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B201" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C201" t="s">
         <v>161</v>
@@ -9832,10 +9835,10 @@
     </row>
     <row r="202" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B202" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C202" t="s">
         <v>161</v>
@@ -9870,10 +9873,10 @@
     </row>
     <row r="203" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B203" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C203" t="s">
         <v>35</v>
@@ -9911,10 +9914,10 @@
     </row>
     <row r="204" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B204" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C204" t="s">
         <v>282</v>
@@ -9952,10 +9955,10 @@
     </row>
     <row r="205" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B205" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C205" t="s">
         <v>282</v>
@@ -9993,10 +9996,10 @@
     </row>
     <row r="206" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B206" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C206" t="s">
         <v>282</v>
@@ -10034,13 +10037,13 @@
     </row>
     <row r="207" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B207" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C207" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D207" t="s">
         <v>29</v>
@@ -10063,13 +10066,13 @@
     </row>
     <row r="208" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B208" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C208" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D208" t="s">
         <v>17</v>
@@ -10092,10 +10095,10 @@
     </row>
     <row r="209" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B209" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D209" t="s">
         <v>29</v>
@@ -10124,10 +10127,10 @@
     </row>
     <row r="210" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B210" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C210" t="s">
         <v>16</v>
@@ -10153,10 +10156,10 @@
     </row>
     <row r="211" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B211" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C211" t="s">
         <v>161</v>
@@ -10182,10 +10185,10 @@
     </row>
     <row r="212" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B212" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C212" t="s">
         <v>161</v>
@@ -10211,10 +10214,10 @@
     </row>
     <row r="213" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B213" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C213" t="s">
         <v>35</v>
@@ -10232,7 +10235,7 @@
         <v>8</v>
       </c>
       <c r="H213" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I213">
         <v>1970</v>
@@ -10252,10 +10255,10 @@
     </row>
     <row r="214" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B214" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C214" t="s">
         <v>161</v>
@@ -10273,7 +10276,7 @@
         <v>8</v>
       </c>
       <c r="H214" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I214" t="s">
         <v>9</v>
@@ -10296,10 +10299,10 @@
     </row>
     <row r="215" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B215" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C215" t="s">
         <v>16</v>
@@ -10317,7 +10320,7 @@
         <v>8</v>
       </c>
       <c r="H215" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I215" t="s">
         <v>9</v>
@@ -10337,10 +10340,10 @@
     </row>
     <row r="216" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B216" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C216" t="s">
         <v>16</v>
@@ -10358,7 +10361,7 @@
         <v>8</v>
       </c>
       <c r="H216" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I216">
         <v>1971</v>
@@ -10378,10 +10381,10 @@
     </row>
     <row r="217" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B217" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C217" t="s">
         <v>16</v>
@@ -10399,7 +10402,7 @@
         <v>8</v>
       </c>
       <c r="H217" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I217">
         <v>1970</v>
@@ -10419,10 +10422,10 @@
     </row>
     <row r="218" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B218" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C218" t="s">
         <v>188</v>
@@ -10440,7 +10443,7 @@
         <v>17</v>
       </c>
       <c r="H218" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I218" t="s">
         <v>9</v>
@@ -10457,10 +10460,10 @@
     </row>
     <row r="219" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B219" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C219" t="s">
         <v>263</v>
@@ -10478,7 +10481,7 @@
         <v>17</v>
       </c>
       <c r="H219" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I219" t="s">
         <v>9</v>
@@ -10495,10 +10498,10 @@
     </row>
     <row r="220" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B220" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C220" t="s">
         <v>161</v>
@@ -10516,7 +10519,7 @@
         <v>8</v>
       </c>
       <c r="H220" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I220">
         <v>2000</v>
@@ -10536,10 +10539,10 @@
     </row>
     <row r="221" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B221" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C221" t="s">
         <v>161</v>
@@ -10557,7 +10560,7 @@
         <v>17</v>
       </c>
       <c r="H221" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I221" t="s">
         <v>9</v>
@@ -10574,10 +10577,10 @@
     </row>
     <row r="222" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B222" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C222" t="s">
         <v>35</v>
@@ -10595,7 +10598,7 @@
         <v>8</v>
       </c>
       <c r="H222" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I222" t="s">
         <v>9</v>
@@ -10615,10 +10618,10 @@
     </row>
     <row r="223" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B223" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C223" t="s">
         <v>282</v>
@@ -10636,7 +10639,7 @@
         <v>8</v>
       </c>
       <c r="H223" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I223" t="s">
         <v>9</v>
@@ -10656,10 +10659,10 @@
     </row>
     <row r="224" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B224" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C224" t="s">
         <v>282</v>
@@ -10677,7 +10680,7 @@
         <v>8</v>
       </c>
       <c r="H224" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I224" t="s">
         <v>9</v>
@@ -10697,10 +10700,10 @@
     </row>
     <row r="225" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B225" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C225" t="s">
         <v>282</v>
@@ -10718,7 +10721,7 @@
         <v>8</v>
       </c>
       <c r="H225" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I225" t="s">
         <v>9</v>
@@ -10738,13 +10741,13 @@
     </row>
     <row r="226" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B226" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C226" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D226" t="s">
         <v>29</v>
@@ -10759,7 +10762,7 @@
         <v>8</v>
       </c>
       <c r="H226" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I226">
         <v>2000</v>
@@ -10773,13 +10776,13 @@
     </row>
     <row r="227" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B227" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C227" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D227" t="s">
         <v>17</v>
@@ -10794,7 +10797,7 @@
         <v>8</v>
       </c>
       <c r="H227" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I227">
         <v>2000</v>
@@ -10808,10 +10811,10 @@
     </row>
     <row r="228" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B228" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D228" t="s">
         <v>29</v>
@@ -10826,7 +10829,7 @@
         <v>8</v>
       </c>
       <c r="H228" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I228" t="s">
         <v>9</v>
@@ -10846,10 +10849,10 @@
     </row>
     <row r="229" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B229" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C229" t="s">
         <v>16</v>
@@ -10867,7 +10870,7 @@
         <v>8</v>
       </c>
       <c r="H229" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K229">
         <v>2000</v>
@@ -10875,10 +10878,10 @@
     </row>
     <row r="230" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B230" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C230" t="s">
         <v>161</v>
@@ -10896,7 +10899,7 @@
         <v>8</v>
       </c>
       <c r="H230" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K230">
         <v>2000</v>
@@ -10904,10 +10907,10 @@
     </row>
     <row r="231" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B231" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C231" t="s">
         <v>161</v>
@@ -10925,7 +10928,7 @@
         <v>8</v>
       </c>
       <c r="H231" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K231">
         <v>2000</v>
@@ -10933,10 +10936,10 @@
     </row>
     <row r="232" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B232" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C232" t="s">
         <v>35</v>
@@ -10954,7 +10957,7 @@
         <v>8</v>
       </c>
       <c r="H232" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I232">
         <v>1970</v>
@@ -10974,10 +10977,10 @@
     </row>
     <row r="233" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B233" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C233" t="s">
         <v>161</v>
@@ -10995,7 +10998,7 @@
         <v>8</v>
       </c>
       <c r="H233" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I233" t="s">
         <v>9</v>
@@ -11018,10 +11021,10 @@
     </row>
     <row r="234" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B234" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C234" t="s">
         <v>16</v>
@@ -11039,7 +11042,7 @@
         <v>8</v>
       </c>
       <c r="H234" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I234" t="s">
         <v>9</v>
@@ -11059,10 +11062,10 @@
     </row>
     <row r="235" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B235" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C235" t="s">
         <v>16</v>
@@ -11080,7 +11083,7 @@
         <v>8</v>
       </c>
       <c r="H235" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I235">
         <v>1971</v>
@@ -11100,10 +11103,10 @@
     </row>
     <row r="236" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B236" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C236" t="s">
         <v>16</v>
@@ -11121,7 +11124,7 @@
         <v>8</v>
       </c>
       <c r="H236" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I236">
         <v>1970</v>
@@ -11141,10 +11144,10 @@
     </row>
     <row r="237" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B237" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C237" t="s">
         <v>188</v>
@@ -11162,7 +11165,7 @@
         <v>17</v>
       </c>
       <c r="H237" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I237" t="s">
         <v>9</v>
@@ -11179,10 +11182,10 @@
     </row>
     <row r="238" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B238" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C238" t="s">
         <v>263</v>
@@ -11200,7 +11203,7 @@
         <v>17</v>
       </c>
       <c r="H238" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I238" t="s">
         <v>9</v>
@@ -11217,10 +11220,10 @@
     </row>
     <row r="239" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B239" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C239" t="s">
         <v>161</v>
@@ -11238,7 +11241,7 @@
         <v>8</v>
       </c>
       <c r="H239" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I239">
         <v>2000</v>
@@ -11258,10 +11261,10 @@
     </row>
     <row r="240" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B240" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C240" t="s">
         <v>161</v>
@@ -11279,7 +11282,7 @@
         <v>17</v>
       </c>
       <c r="H240" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I240" t="s">
         <v>9</v>
@@ -11296,10 +11299,10 @@
     </row>
     <row r="241" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B241" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C241" t="s">
         <v>35</v>
@@ -11317,7 +11320,7 @@
         <v>8</v>
       </c>
       <c r="H241" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I241" t="s">
         <v>9</v>
@@ -11337,10 +11340,10 @@
     </row>
     <row r="242" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B242" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C242" t="s">
         <v>282</v>
@@ -11358,7 +11361,7 @@
         <v>8</v>
       </c>
       <c r="H242" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I242" t="s">
         <v>9</v>
@@ -11378,10 +11381,10 @@
     </row>
     <row r="243" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B243" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C243" t="s">
         <v>282</v>
@@ -11399,7 +11402,7 @@
         <v>8</v>
       </c>
       <c r="H243" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I243" t="s">
         <v>9</v>
@@ -11419,10 +11422,10 @@
     </row>
     <row r="244" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B244" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C244" t="s">
         <v>282</v>
@@ -11440,7 +11443,7 @@
         <v>8</v>
       </c>
       <c r="H244" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I244" t="s">
         <v>9</v>
@@ -11460,13 +11463,13 @@
     </row>
     <row r="245" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B245" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C245" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D245" t="s">
         <v>29</v>
@@ -11481,7 +11484,7 @@
         <v>8</v>
       </c>
       <c r="H245" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I245">
         <v>2000</v>
@@ -11495,13 +11498,13 @@
     </row>
     <row r="246" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B246" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C246" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D246" t="s">
         <v>17</v>
@@ -11516,7 +11519,7 @@
         <v>8</v>
       </c>
       <c r="H246" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I246">
         <v>2000</v>
@@ -11530,10 +11533,10 @@
     </row>
     <row r="247" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B247" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D247" t="s">
         <v>29</v>
@@ -11548,7 +11551,7 @@
         <v>8</v>
       </c>
       <c r="H247" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I247" t="s">
         <v>9</v>
@@ -11568,10 +11571,10 @@
     </row>
     <row r="248" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B248" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C248" t="s">
         <v>16</v>
@@ -11589,7 +11592,7 @@
         <v>8</v>
       </c>
       <c r="H248" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K248">
         <v>2000</v>
@@ -11597,10 +11600,10 @@
     </row>
     <row r="249" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B249" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C249" t="s">
         <v>161</v>
@@ -11618,7 +11621,7 @@
         <v>8</v>
       </c>
       <c r="H249" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K249">
         <v>2000</v>
@@ -11626,10 +11629,10 @@
     </row>
     <row r="250" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B250" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C250" t="s">
         <v>161</v>
@@ -11647,7 +11650,7 @@
         <v>8</v>
       </c>
       <c r="H250" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K250">
         <v>2000</v>
@@ -11655,10 +11658,10 @@
     </row>
     <row r="251" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B251" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C251" t="s">
         <v>35</v>
@@ -11676,7 +11679,7 @@
         <v>8</v>
       </c>
       <c r="H251" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I251">
         <v>1970</v>
@@ -11696,10 +11699,10 @@
     </row>
     <row r="252" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B252" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C252" t="s">
         <v>161</v>
@@ -11717,7 +11720,7 @@
         <v>8</v>
       </c>
       <c r="H252" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I252" t="s">
         <v>9</v>
@@ -11740,10 +11743,10 @@
     </row>
     <row r="253" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B253" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C253" t="s">
         <v>16</v>
@@ -11761,7 +11764,7 @@
         <v>8</v>
       </c>
       <c r="H253" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I253" t="s">
         <v>9</v>
@@ -11781,10 +11784,10 @@
     </row>
     <row r="254" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B254" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C254" t="s">
         <v>16</v>
@@ -11802,7 +11805,7 @@
         <v>8</v>
       </c>
       <c r="H254" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I254">
         <v>1971</v>
@@ -11822,10 +11825,10 @@
     </row>
     <row r="255" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B255" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C255" t="s">
         <v>16</v>
@@ -11843,7 +11846,7 @@
         <v>8</v>
       </c>
       <c r="H255" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I255">
         <v>1970</v>
@@ -11863,10 +11866,10 @@
     </row>
     <row r="256" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B256" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C256" t="s">
         <v>188</v>
@@ -11884,7 +11887,7 @@
         <v>17</v>
       </c>
       <c r="H256" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I256" t="s">
         <v>9</v>
@@ -11901,10 +11904,10 @@
     </row>
     <row r="257" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B257" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C257" t="s">
         <v>263</v>
@@ -11922,7 +11925,7 @@
         <v>17</v>
       </c>
       <c r="H257" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I257" t="s">
         <v>9</v>
@@ -11939,10 +11942,10 @@
     </row>
     <row r="258" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B258" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C258" t="s">
         <v>161</v>
@@ -11960,7 +11963,7 @@
         <v>8</v>
       </c>
       <c r="H258" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I258">
         <v>2000</v>
@@ -11980,10 +11983,10 @@
     </row>
     <row r="259" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B259" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C259" t="s">
         <v>161</v>
@@ -12001,7 +12004,7 @@
         <v>17</v>
       </c>
       <c r="H259" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I259" t="s">
         <v>9</v>
@@ -12018,10 +12021,10 @@
     </row>
     <row r="260" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B260" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C260" t="s">
         <v>35</v>
@@ -12039,7 +12042,7 @@
         <v>8</v>
       </c>
       <c r="H260" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I260" t="s">
         <v>9</v>
@@ -12059,10 +12062,10 @@
     </row>
     <row r="261" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B261" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C261" t="s">
         <v>282</v>
@@ -12080,7 +12083,7 @@
         <v>8</v>
       </c>
       <c r="H261" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I261" t="s">
         <v>9</v>
@@ -12100,10 +12103,10 @@
     </row>
     <row r="262" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B262" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C262" t="s">
         <v>282</v>
@@ -12121,7 +12124,7 @@
         <v>8</v>
       </c>
       <c r="H262" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I262" t="s">
         <v>9</v>
@@ -12141,10 +12144,10 @@
     </row>
     <row r="263" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B263" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C263" t="s">
         <v>282</v>
@@ -12162,7 +12165,7 @@
         <v>8</v>
       </c>
       <c r="H263" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I263" t="s">
         <v>9</v>
@@ -12182,13 +12185,13 @@
     </row>
     <row r="264" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B264" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C264" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D264" t="s">
         <v>29</v>
@@ -12203,7 +12206,7 @@
         <v>8</v>
       </c>
       <c r="H264" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I264">
         <v>2000</v>
@@ -12217,13 +12220,13 @@
     </row>
     <row r="265" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B265" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C265" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D265" t="s">
         <v>17</v>
@@ -12238,7 +12241,7 @@
         <v>8</v>
       </c>
       <c r="H265" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I265">
         <v>2000</v>
@@ -12252,10 +12255,10 @@
     </row>
     <row r="266" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B266" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D266" t="s">
         <v>29</v>
@@ -12270,7 +12273,7 @@
         <v>8</v>
       </c>
       <c r="H266" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I266" t="s">
         <v>9</v>
@@ -12290,10 +12293,10 @@
     </row>
     <row r="267" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B267" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C267" t="s">
         <v>16</v>
@@ -12311,7 +12314,7 @@
         <v>8</v>
       </c>
       <c r="H267" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="K267">
         <v>2000</v>
@@ -12319,10 +12322,10 @@
     </row>
     <row r="268" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B268" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C268" t="s">
         <v>161</v>
@@ -12340,7 +12343,7 @@
         <v>8</v>
       </c>
       <c r="H268" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="K268">
         <v>2000</v>
@@ -12348,10 +12351,10 @@
     </row>
     <row r="269" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B269" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C269" t="s">
         <v>161</v>
@@ -12369,7 +12372,7 @@
         <v>8</v>
       </c>
       <c r="H269" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="K269">
         <v>2000</v>
@@ -12377,10 +12380,10 @@
     </row>
     <row r="270" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B270" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C270" t="s">
         <v>35</v>
@@ -12398,7 +12401,7 @@
         <v>8</v>
       </c>
       <c r="H270" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I270">
         <v>1970</v>
@@ -12418,10 +12421,10 @@
     </row>
     <row r="271" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B271" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C271" t="s">
         <v>161</v>
@@ -12439,7 +12442,7 @@
         <v>8</v>
       </c>
       <c r="H271" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I271" t="s">
         <v>9</v>
@@ -12462,10 +12465,10 @@
     </row>
     <row r="272" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B272" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C272" t="s">
         <v>16</v>
@@ -12483,7 +12486,7 @@
         <v>8</v>
       </c>
       <c r="H272" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I272" t="s">
         <v>9</v>
@@ -12503,10 +12506,10 @@
     </row>
     <row r="273" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B273" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C273" t="s">
         <v>16</v>
@@ -12524,7 +12527,7 @@
         <v>8</v>
       </c>
       <c r="H273" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I273">
         <v>1971</v>
@@ -12544,10 +12547,10 @@
     </row>
     <row r="274" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B274" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C274" t="s">
         <v>16</v>
@@ -12565,7 +12568,7 @@
         <v>8</v>
       </c>
       <c r="H274" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I274">
         <v>1970</v>
@@ -12585,10 +12588,10 @@
     </row>
     <row r="275" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B275" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C275" t="s">
         <v>188</v>
@@ -12606,7 +12609,7 @@
         <v>17</v>
       </c>
       <c r="H275" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I275" t="s">
         <v>9</v>
@@ -12623,10 +12626,10 @@
     </row>
     <row r="276" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B276" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C276" t="s">
         <v>263</v>
@@ -12644,7 +12647,7 @@
         <v>17</v>
       </c>
       <c r="H276" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I276" t="s">
         <v>9</v>
@@ -12661,10 +12664,10 @@
     </row>
     <row r="277" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B277" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C277" t="s">
         <v>161</v>
@@ -12682,7 +12685,7 @@
         <v>8</v>
       </c>
       <c r="H277" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I277">
         <v>2000</v>
@@ -12702,10 +12705,10 @@
     </row>
     <row r="278" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B278" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C278" t="s">
         <v>161</v>
@@ -12723,7 +12726,7 @@
         <v>17</v>
       </c>
       <c r="H278" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I278" t="s">
         <v>9</v>
@@ -12740,10 +12743,10 @@
     </row>
     <row r="279" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B279" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C279" t="s">
         <v>35</v>
@@ -12761,7 +12764,7 @@
         <v>8</v>
       </c>
       <c r="H279" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I279" t="s">
         <v>9</v>
@@ -12781,10 +12784,10 @@
     </row>
     <row r="280" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B280" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C280" t="s">
         <v>282</v>
@@ -12802,7 +12805,7 @@
         <v>8</v>
       </c>
       <c r="H280" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I280" t="s">
         <v>9</v>
@@ -12822,10 +12825,10 @@
     </row>
     <row r="281" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B281" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C281" t="s">
         <v>282</v>
@@ -12843,7 +12846,7 @@
         <v>8</v>
       </c>
       <c r="H281" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I281" t="s">
         <v>9</v>
@@ -12863,10 +12866,10 @@
     </row>
     <row r="282" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B282" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C282" t="s">
         <v>282</v>
@@ -12884,7 +12887,7 @@
         <v>8</v>
       </c>
       <c r="H282" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I282" t="s">
         <v>9</v>
@@ -12904,13 +12907,13 @@
     </row>
     <row r="283" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B283" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C283" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D283" t="s">
         <v>29</v>
@@ -12925,7 +12928,7 @@
         <v>8</v>
       </c>
       <c r="H283" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I283">
         <v>2000</v>
@@ -12939,13 +12942,13 @@
     </row>
     <row r="284" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B284" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C284" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D284" t="s">
         <v>17</v>
@@ -12960,7 +12963,7 @@
         <v>8</v>
       </c>
       <c r="H284" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I284">
         <v>2000</v>
@@ -12974,10 +12977,10 @@
     </row>
     <row r="285" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B285" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D285" t="s">
         <v>29</v>
@@ -12992,7 +12995,7 @@
         <v>8</v>
       </c>
       <c r="H285" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I285" t="s">
         <v>9</v>
@@ -13012,10 +13015,10 @@
     </row>
     <row r="286" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B286" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C286" t="s">
         <v>16</v>
@@ -13033,7 +13036,7 @@
         <v>8</v>
       </c>
       <c r="H286" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K286">
         <v>2000</v>
@@ -13041,10 +13044,10 @@
     </row>
     <row r="287" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B287" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C287" t="s">
         <v>161</v>
@@ -13062,7 +13065,7 @@
         <v>8</v>
       </c>
       <c r="H287" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K287">
         <v>2000</v>
@@ -13070,10 +13073,10 @@
     </row>
     <row r="288" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B288" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C288" t="s">
         <v>161</v>
@@ -13091,7 +13094,7 @@
         <v>8</v>
       </c>
       <c r="H288" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K288">
         <v>2000</v>
@@ -13143,7 +13146,7 @@
         <v>409</v>
       </c>
       <c r="C290" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D290" t="s">
         <v>29</v>
@@ -13843,7 +13846,7 @@
         <v>455</v>
       </c>
       <c r="C310" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D310" t="s">
         <v>29</v>
@@ -14003,7 +14006,7 @@
         <v>466</v>
       </c>
       <c r="C315" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D315" t="s">
         <v>29</v>
@@ -14038,7 +14041,7 @@
         <v>468</v>
       </c>
       <c r="C316" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D316" t="s">
         <v>29</v>
@@ -14073,7 +14076,7 @@
         <v>470</v>
       </c>
       <c r="C317" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D317" t="s">
         <v>29</v>
@@ -14108,7 +14111,7 @@
         <v>472</v>
       </c>
       <c r="C318" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D318" t="s">
         <v>29</v>
@@ -14143,7 +14146,7 @@
         <v>474</v>
       </c>
       <c r="C319" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D319" t="s">
         <v>29</v>
@@ -14178,7 +14181,7 @@
         <v>476</v>
       </c>
       <c r="C320" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D320" t="s">
         <v>29</v>
@@ -14210,10 +14213,10 @@
         <v>482</v>
       </c>
       <c r="B321" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C321" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D321" t="s">
         <v>29</v>
@@ -14347,10 +14350,10 @@
         <v>489</v>
       </c>
       <c r="B325" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C325" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D325" t="s">
         <v>29</v>
@@ -14382,10 +14385,10 @@
         <v>490</v>
       </c>
       <c r="B326" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C326" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D326" t="s">
         <v>29</v>
@@ -14417,10 +14420,10 @@
         <v>491</v>
       </c>
       <c r="B327" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C327" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D327" t="s">
         <v>29</v>
@@ -14487,10 +14490,10 @@
         <v>494</v>
       </c>
       <c r="B329" t="s">
-        <v>495</v>
+        <v>739</v>
       </c>
       <c r="C329" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D329" t="s">
         <v>29</v>
@@ -14519,13 +14522,13 @@
     </row>
     <row r="330" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
+        <v>592</v>
+      </c>
+      <c r="B330" t="s">
         <v>593</v>
       </c>
-      <c r="B330" t="s">
-        <v>594</v>
-      </c>
       <c r="C330" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D330" t="s">
         <v>17</v>
@@ -14554,13 +14557,13 @@
     </row>
     <row r="331" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B331" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C331" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D331" t="s">
         <v>29</v>
@@ -14589,10 +14592,10 @@
     </row>
     <row r="332" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B332" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D332" t="s">
         <v>17</v>

</xml_diff>